<commit_message>
Update script and inputs for new cadre calculations
Delete: Run_simulations_new.R and model_inputs_shiny_demo.xlsx were used for testing purposes only.
Update: Run_simulations.R, model_inputs_demo.xlsx
Add: Analysis_pipeline_demo.R
</commit_message>
<xml_diff>
--- a/config/model_inputs_demo.xlsx
+++ b/config/model_inputs_demo.xlsx
@@ -8,39 +8,46 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/rui_han_gatesfoundation_org/Documents/Documents/GitHub/Ethiopia-HEP-Capacity-Analysis/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="253" documentId="13_ncr:1_{7CCCDFD1-E59D-423C-8BB5-C2031FD3030E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D644CFF-4A1D-4FD1-AE44-D50D53B1EDB9}"/>
+  <xr:revisionPtr revIDLastSave="286" documentId="13_ncr:1_{7CCCDFD1-E59D-423C-8BB5-C2031FD3030E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{759DB3FD-D57C-4A43-97B2-53A3A60D15C6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="830" firstSheet="4" activeTab="11" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
+    <workbookView xWindow="6390" yWindow="-21030" windowWidth="32880" windowHeight="18390" tabRatio="830" activeTab="12" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="77" r:id="rId1"/>
     <sheet name="Scenarios" sheetId="53" r:id="rId2"/>
     <sheet name="PopValues" sheetId="102" r:id="rId3"/>
-    <sheet name="TotalPop" sheetId="54" r:id="rId4"/>
-    <sheet name="RuralPop" sheetId="110" r:id="rId5"/>
-    <sheet name="StochasticParameters" sheetId="72" r:id="rId6"/>
-    <sheet name="SeasonalityCurves" sheetId="58" r:id="rId7"/>
-    <sheet name="SeasonalityOffsets" sheetId="66" r:id="rId8"/>
-    <sheet name="TaskValues_basic" sheetId="83" r:id="rId9"/>
-    <sheet name="TaskValues_expanded" sheetId="109" r:id="rId10"/>
-    <sheet name="Cadres" sheetId="97" r:id="rId11"/>
-    <sheet name="CadreRoles" sheetId="111" r:id="rId12"/>
-    <sheet name="CadreRoles_v0" sheetId="108" r:id="rId13"/>
-    <sheet name="Data dictionary Scenarios" sheetId="63" r:id="rId14"/>
-    <sheet name="Lookup" sheetId="84" r:id="rId15"/>
+    <sheet name="ChangeRateLimits" sheetId="112" r:id="rId4"/>
+    <sheet name="TotalPop" sheetId="54" r:id="rId5"/>
+    <sheet name="RuralPop" sheetId="110" r:id="rId6"/>
+    <sheet name="StochasticParameters" sheetId="72" r:id="rId7"/>
+    <sheet name="SeasonalityCurves" sheetId="58" r:id="rId8"/>
+    <sheet name="SeasonalityOffsets" sheetId="66" r:id="rId9"/>
+    <sheet name="TaskValues_basic" sheetId="83" r:id="rId10"/>
+    <sheet name="TaskValues_expanded" sheetId="109" r:id="rId11"/>
+    <sheet name="TaskAllocationByCadre" sheetId="97" r:id="rId12"/>
+    <sheet name="CadreRoles" sheetId="111" r:id="rId13"/>
+    <sheet name="CadreRoles_v0" sheetId="108" r:id="rId14"/>
+    <sheet name="Data dictionary Scenarios" sheetId="63" r:id="rId15"/>
+    <sheet name="Lookup" sheetId="84" r:id="rId16"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">TaskValues_basic!$B$1:$Q$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TaskValues_expanded!$B$1:$P$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TaskValues_basic!$B$1:$Q$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">TaskValues_expanded!$B$1:$P$22</definedName>
+    <definedName name="hours" localSheetId="3">#REF!</definedName>
     <definedName name="hours">#REF!</definedName>
+    <definedName name="select_pop" localSheetId="3">#REF!</definedName>
     <definedName name="select_pop">#REF!</definedName>
-    <definedName name="total_pop" localSheetId="4">RuralPop!#REF!</definedName>
-    <definedName name="total_pop" localSheetId="3">TotalPop!#REF!</definedName>
+    <definedName name="total_pop" localSheetId="3">#REF!</definedName>
+    <definedName name="total_pop" localSheetId="5">RuralPop!#REF!</definedName>
+    <definedName name="total_pop" localSheetId="4">TotalPop!#REF!</definedName>
     <definedName name="total_pop">#REF!</definedName>
-    <definedName name="total_pop2">[1]Demographics_Total!$CZ$3</definedName>
+    <definedName name="total_pop2" localSheetId="3">[1]Demographics_Total!$CZ$3</definedName>
+    <definedName name="total_pop2">[2]Demographics_Total!$CZ$3</definedName>
+    <definedName name="weeks" localSheetId="3">#REF!</definedName>
     <definedName name="weeks">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -169,8 +176,66 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Rui Han (AgileOne)</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{15E9D0E6-7E00-496C-82F5-4E3CFF13E51F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rui Han (AgileOne):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The category of rates the limits apply to</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{01EB944C-05CF-4CC3-85DD-3C9FF8700F6A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rui Han (AgileOne):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Values are ratio to baseline rates
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="324">
   <si>
     <t>Pregnancy</t>
   </si>
@@ -1042,9 +1107,6 @@
     <t>Annualized DHS rate</t>
   </si>
   <si>
-    <t>Cadres</t>
-  </si>
-  <si>
     <t>Hyper1524</t>
   </si>
   <si>
@@ -1117,19 +1179,34 @@
     <t>DESC_col</t>
   </si>
   <si>
-    <t>Format update date: 5/25/2023.</t>
-  </si>
-  <si>
     <t>Version 2.1 of the model_inputs_demo.xlsx file.</t>
   </si>
   <si>
-    <t>Works with code versions up through at least 2.0? Not compatible with pacehrh versions 1.0.6 and earlier.</t>
-  </si>
-  <si>
     <t>OverheadHoursPerWeek</t>
   </si>
   <si>
     <t>Family health professional</t>
+  </si>
+  <si>
+    <t>TaskAllocationByCadre</t>
+  </si>
+  <si>
+    <t>RateCategory</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Incidence</t>
+  </si>
+  <si>
+    <t>Works with code versions up through at least 1.0.7.  Not compatible with pacehrh versions 1.0.6 and earlier.</t>
+  </si>
+  <si>
+    <t>Format update date: 6/2/2023.</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1221,7 @@
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1266,6 +1343,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1317,7 +1407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1425,8 +1515,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1440,8 +1581,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1570,9 +1712,27 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="12" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="13" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="14" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="11" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="10" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="9" xr:uid="{F410D60A-1DC9-43C7-979B-E919CC121327}"/>
     <cellStyle name="Data" xfId="6" xr:uid="{210BAF51-33D3-495B-9156-CBDCF2D0412F}"/>
     <cellStyle name="Header" xfId="5" xr:uid="{3562FB01-884A-4428-8FB5-9312164FC171}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1660,6 +1820,149 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="To Do or Upgrade"/>
+      <sheetName val="Inputs Assump"/>
+      <sheetName val="C FTE Equiv"/>
+      <sheetName val="C Tot Hrs by Cat"/>
+      <sheetName val="C Variance"/>
+      <sheetName val="Time Summary"/>
+      <sheetName val="C Hrs by Category (3)"/>
+      <sheetName val="C Hrs by Category (2)"/>
+      <sheetName val="C Ratio to Baseline"/>
+      <sheetName val="Pie 2020"/>
+      <sheetName val="Calculations"/>
+      <sheetName val="Demographics_InCalc"/>
+      <sheetName val="Births"/>
+      <sheetName val="Mortality"/>
+      <sheetName val="FH.MC"/>
+      <sheetName val="FH.FP"/>
+      <sheetName val="FH.Im"/>
+      <sheetName val="FH.N"/>
+      <sheetName val="DPC"/>
+      <sheetName val="Other"/>
+      <sheetName val="DATA"/>
+      <sheetName val="Ssn Malaria"/>
+      <sheetName val="Ssn Nutr"/>
+      <sheetName val="Ssn Measles"/>
+      <sheetName val="Demographics_Total"/>
+      <sheetName val="Prevalences"/>
+      <sheetName val="Work time"/>
+      <sheetName val="Sheet21"/>
+      <sheetName val="Services summary"/>
+      <sheetName val="Services ref"/>
+      <sheetName val="Coverage impacts"/>
+      <sheetName val="Pop M"/>
+      <sheetName val="Pop F"/>
+      <sheetName val="TB Incidence"/>
+      <sheetName val="Malaria Incid"/>
+      <sheetName val="C Fertility"/>
+      <sheetName val="fertility"/>
+      <sheetName val="FP mod"/>
+      <sheetName val="unmet need"/>
+      <sheetName val="HIV Prev"/>
+      <sheetName val="HIV Incid"/>
+      <sheetName val="mort infant"/>
+      <sheetName val="mort 1-5"/>
+      <sheetName val="mort 5-9"/>
+      <sheetName val="mort 10-14"/>
+      <sheetName val="mort 15-19"/>
+      <sheetName val="mort 20-24"/>
+      <sheetName val="mort adult f"/>
+      <sheetName val="mort adult m"/>
+      <sheetName val="Staffing Ratios"/>
+      <sheetName val="fertility 15-19"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="4">
+          <cell r="C4" t="str">
+            <v>Ratio max rural</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11">
+        <row r="4">
+          <cell r="V4">
+            <v>105.34416988791497</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24">
+        <row r="3">
+          <cell r="CZ3">
+            <v>115103531.71799999</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39">
+        <row r="77">
+          <cell r="BC77">
+            <v>1.4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="40">
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>Ethiopia</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2149,19 +2452,19 @@
   <dimension ref="B2:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="P3" s="28" t="b">
         <v>1</v>
@@ -2175,7 +2478,7 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="P4" s="28" t="b">
         <v>0</v>
@@ -2223,15 +2526,740 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9F8961-463F-4540-AE96-5FF353928741}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:Q16"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.90625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1796875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18.7265625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="16" customFormat="1" ht="87.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="43" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="48" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="52" t="s">
+        <v>279</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="57">
+        <v>1</v>
+      </c>
+      <c r="I2" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="58"/>
+      <c r="L2" s="58">
+        <v>1</v>
+      </c>
+      <c r="M2" s="59">
+        <v>4</v>
+      </c>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59">
+        <v>10</v>
+      </c>
+      <c r="P2" s="59"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="60">
+        <v>1</v>
+      </c>
+      <c r="I3" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="24"/>
+      <c r="L3" s="24">
+        <v>1</v>
+      </c>
+      <c r="M3" s="62">
+        <v>2</v>
+      </c>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62">
+        <v>30</v>
+      </c>
+      <c r="P3" s="62"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="60">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="24"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="24">
+        <v>1</v>
+      </c>
+      <c r="M4" s="62">
+        <v>3</v>
+      </c>
+      <c r="N4" s="62"/>
+      <c r="O4" s="63">
+        <v>5</v>
+      </c>
+      <c r="P4" s="63"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="60">
+        <v>1</v>
+      </c>
+      <c r="I5" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="24"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="24">
+        <v>1</v>
+      </c>
+      <c r="M5" s="62">
+        <v>4</v>
+      </c>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62">
+        <v>5</v>
+      </c>
+      <c r="P5" s="62"/>
+    </row>
+    <row r="6" spans="1:17" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>266</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="67" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="69">
+        <v>1</v>
+      </c>
+      <c r="I6" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="71"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="71">
+        <v>1</v>
+      </c>
+      <c r="M6" s="72">
+        <v>1</v>
+      </c>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72">
+        <v>5</v>
+      </c>
+      <c r="P6" s="72"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="39">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="I7" t="s">
+        <v>289</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42">
+        <v>0.98</v>
+      </c>
+      <c r="M7" s="40">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8"/>
+      <c r="O7" s="40">
+        <v>5</v>
+      </c>
+      <c r="P7" s="40"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="39">
+        <v>0.46090000000000003</v>
+      </c>
+      <c r="I8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42">
+        <v>0.98</v>
+      </c>
+      <c r="M8" s="40">
+        <v>2</v>
+      </c>
+      <c r="N8" s="8"/>
+      <c r="O8" s="40">
+        <v>5</v>
+      </c>
+      <c r="P8" s="40"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="C9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="39">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="I9" t="s">
+        <v>148</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="42">
+        <v>0.98</v>
+      </c>
+      <c r="M9" s="40">
+        <v>2</v>
+      </c>
+      <c r="N9" s="8"/>
+      <c r="O9" s="40">
+        <v>5</v>
+      </c>
+      <c r="P9" s="40"/>
+    </row>
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="39">
+        <v>0.27813253012048195</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="9">
+        <v>1</v>
+      </c>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8">
+        <v>4</v>
+      </c>
+      <c r="O10" s="8">
+        <v>5</v>
+      </c>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="52" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="53" t="s">
+        <v>268</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>285</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="57">
+        <v>2.0927000000000001E-4</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>286</v>
+      </c>
+      <c r="J11" s="58">
+        <v>4</v>
+      </c>
+      <c r="K11" s="54" t="s">
+        <v>276</v>
+      </c>
+      <c r="L11" s="58">
+        <v>0.90986310592664843</v>
+      </c>
+      <c r="M11" s="59">
+        <v>1</v>
+      </c>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59">
+        <v>5</v>
+      </c>
+      <c r="P11" s="59"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="C12" t="s">
+        <v>282</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="73">
+        <v>3.6788000000000001E-2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>148</v>
+      </c>
+      <c r="J12" s="24">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
+        <v>276</v>
+      </c>
+      <c r="L12" s="24">
+        <v>1</v>
+      </c>
+      <c r="M12" s="62">
+        <v>1</v>
+      </c>
+      <c r="N12" s="62"/>
+      <c r="O12" s="62">
+        <v>5</v>
+      </c>
+      <c r="P12" s="62"/>
+    </row>
+    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>281</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="C13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="H13" s="39">
+        <v>4.7E-2</v>
+      </c>
+      <c r="I13" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="K13" s="41" t="s">
+        <v>277</v>
+      </c>
+      <c r="L13" s="9">
+        <v>1</v>
+      </c>
+      <c r="M13" s="8">
+        <v>2</v>
+      </c>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8">
+        <v>10</v>
+      </c>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="52" t="s">
+        <v>287</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>272</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="57">
+        <v>3.3109200000000005E-2</v>
+      </c>
+      <c r="I14" s="54" t="s">
+        <v>148</v>
+      </c>
+      <c r="J14" s="58"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="58">
+        <v>0.87556301899925537</v>
+      </c>
+      <c r="M14" s="59">
+        <v>1</v>
+      </c>
+      <c r="N14" s="59"/>
+      <c r="O14" s="59">
+        <v>10</v>
+      </c>
+      <c r="P14" s="59"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="60">
+        <v>3.3109200000000005E-2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>148</v>
+      </c>
+      <c r="J15" s="24"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="24">
+        <v>0.87556301899925537</v>
+      </c>
+      <c r="M15" s="62">
+        <v>1</v>
+      </c>
+      <c r="N15" s="62"/>
+      <c r="O15" s="62">
+        <v>10</v>
+      </c>
+      <c r="P15" s="62"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="J16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1E3EE0E1-6392-4754-984C-80D83AFED092}">
+          <x14:formula1>
+            <xm:f>Lookup!$D$2:$D$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F9 F11:F15 F17:F332</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{925A0EEB-9365-4265-BCAA-8FCF4189DF40}">
+          <x14:formula1>
+            <xm:f>Lookup!$B$2:$B$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E15 E17:E233</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C319048F-06A6-4121-9C15-D4FC96370093}">
+          <x14:formula1>
+            <xm:f>Lookup!$F$2:$F$45</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G15 G17:G1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE02F26-882B-45E6-A19E-6B7248DFCF45}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2780,7 +3808,7 @@
         <v>281</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C13" t="s">
         <v>158</v>
@@ -2910,7 +3938,7 @@
         <v>287</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C16" t="s">
         <v>249</v>
@@ -2952,7 +3980,7 @@
         <v>287</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C17" t="s">
         <v>250</v>
@@ -2994,7 +4022,7 @@
         <v>287</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C18" t="s">
         <v>251</v>
@@ -3036,7 +4064,7 @@
         <v>287</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C19" t="s">
         <v>252</v>
@@ -3078,7 +4106,7 @@
         <v>287</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C20" t="s">
         <v>253</v>
@@ -3120,7 +4148,7 @@
         <v>287</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C21" s="66" t="s">
         <v>254</v>
@@ -3300,16 +4328,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04D6E33-24B9-46AB-8C0C-B9AE70A8D6D8}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S20" sqref="S20"/>
+      <selection pane="bottomLeft" activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3317,7 +4345,7 @@
     <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.08984375" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" style="23" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.81640625" style="23" bestFit="1" customWidth="1"/>
@@ -3329,10 +4357,10 @@
   <sheetData>
     <row r="1" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="85" t="s">
+        <v>312</v>
+      </c>
+      <c r="B1" s="87" t="s">
         <v>313</v>
-      </c>
-      <c r="B1" s="87" t="s">
-        <v>314</v>
       </c>
       <c r="C1" s="88" t="str">
         <f>_xlfn.CONCAT("StartYear", 2020)</f>
@@ -3399,43 +4427,43 @@
         <v>37</v>
       </c>
       <c r="C2" s="90" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D2" s="90" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E2" s="91" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="90" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G2" s="90" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H2" s="91" t="s">
         <v>34</v>
       </c>
       <c r="I2" s="90" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J2" s="90" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K2" s="90" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L2" s="91" t="s">
         <v>34</v>
       </c>
       <c r="M2" s="90" t="s">
+        <v>305</v>
+      </c>
+      <c r="N2" s="90" t="s">
         <v>306</v>
       </c>
-      <c r="N2" s="90" t="s">
-        <v>307</v>
-      </c>
       <c r="O2" s="90" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P2" s="91" t="s">
         <v>34</v>
@@ -4048,7 +5076,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B14" t="str">
         <f>VLOOKUP(A14,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -4213,7 +5241,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B17" t="str">
         <f>VLOOKUP(A17,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -4268,7 +5296,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B18" t="str">
         <f>VLOOKUP(A18,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -4323,7 +5351,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B19" t="str">
         <f>VLOOKUP(A19,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -4378,7 +5406,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B20" t="str">
         <f>VLOOKUP(A20,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -4433,7 +5461,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B21" t="str">
         <f>VLOOKUP(A21,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -4488,7 +5516,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP(A22,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -4680,15 +5708,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A266884E-25A4-43DE-83DF-867907ACC671}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4703,16 +5731,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="82" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="C1" s="82" t="s">
         <v>304</v>
       </c>
-      <c r="C1" s="82" t="s">
-        <v>305</v>
-      </c>
       <c r="D1" s="82" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E1" s="82" t="s">
         <v>247</v>
@@ -4723,13 +5751,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D2" s="22">
         <v>5</v>
@@ -4743,13 +5771,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D3" s="22">
         <v>5</v>
@@ -4761,13 +5789,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D4" s="22">
         <v>5</v>
@@ -4782,10 +5810,10 @@
         <v>258</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>311</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>312</v>
       </c>
       <c r="D5" s="22">
         <v>5</v>
@@ -4802,10 +5830,10 @@
         <v>258</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D6" s="22">
         <v>5</v>
@@ -4820,10 +5848,10 @@
         <v>258</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D7" s="22">
         <v>5</v>
@@ -4835,13 +5863,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D8" s="22">
         <v>5</v>
@@ -4855,13 +5883,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D9" s="22">
         <v>5</v>
@@ -4873,13 +5901,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D10" s="22">
         <v>5</v>
@@ -4916,7 +5944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54E086A-5AFA-4FBE-A195-2972B691F429}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -4939,16 +5967,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="82" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="C1" s="82" t="s">
         <v>304</v>
       </c>
-      <c r="C1" s="82" t="s">
-        <v>305</v>
-      </c>
       <c r="D1" s="82" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E1" s="82" t="s">
         <v>247</v>
@@ -4959,13 +5987,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -4979,13 +6007,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D3" s="22">
         <v>4</v>
@@ -4997,13 +6025,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D4" s="22">
         <v>4</v>
@@ -5018,10 +6046,10 @@
         <v>258</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>311</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>312</v>
       </c>
       <c r="D5" s="22">
         <v>4.5</v>
@@ -5038,10 +6066,10 @@
         <v>258</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D6" s="22">
         <v>5.5</v>
@@ -5056,10 +6084,10 @@
         <v>258</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D7" s="22">
         <v>5.5</v>
@@ -5071,13 +6099,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D8" s="22">
         <v>3</v>
@@ -5091,13 +6119,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D9" s="22">
         <v>4</v>
@@ -5109,13 +6137,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D10" s="22">
         <v>4</v>
@@ -5152,7 +6180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88F02ED-B255-4EEF-8CAA-1A7122B8C9FB}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -5282,12 +6310,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2681DF91-CB0A-43E1-9090-E7803F99E625}">
   <dimension ref="B1:L142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5323,7 +6351,7 @@
         <v>176</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
@@ -5349,7 +6377,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
@@ -5375,7 +6403,7 @@
         <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
@@ -5401,7 +6429,7 @@
         <v>9</v>
       </c>
       <c r="L4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -5427,7 +6455,7 @@
         <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
@@ -6409,7 +7437,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6424,7 +7452,7 @@
     <col min="9" max="9" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="84" customFormat="1" ht="112" customHeight="1" x14ac:dyDescent="0.35">
@@ -6468,7 +7496,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B2" s="27">
         <v>48</v>
@@ -6495,13 +7523,13 @@
         <v>256</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>143</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>290</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -6533,18 +7561,18 @@
         <v>257</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>143</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>290</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B4" s="27">
         <v>48</v>
@@ -6571,13 +7599,13 @@
         <v>256</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>143</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>290</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -6632,7 +7660,7 @@
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:L4 A2:A4" xr:uid="{87300A30-10E8-4D88-9E37-E7127D8D74E3}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4 I2:L4" xr:uid="{87300A30-10E8-4D88-9E37-E7127D8D74E3}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -7518,6 +8546,73 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5EA865-0CD0-41A0-8D11-2E731D20BD4F}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.90625" customWidth="1"/>
+    <col min="2" max="3" width="5.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="92" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" s="93" t="s">
+        <v>319</v>
+      </c>
+      <c r="C1" s="94" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="95" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="96">
+        <v>0.6</v>
+      </c>
+      <c r="C2" s="97">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="95" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="98">
+        <v>0.8</v>
+      </c>
+      <c r="C3" s="99">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="100" t="s">
+        <v>321</v>
+      </c>
+      <c r="B4" s="101">
+        <v>0.75</v>
+      </c>
+      <c r="C4" s="102">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F96BBDE-B309-4A5A-8E01-1740FFC9B513}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -7525,7 +8620,7 @@
   <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8978,7 +10073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F290AA6-1CD3-431F-9AA8-6DFC42821499}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -10439,7 +11534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDCD1CB-9612-4FAF-ACD4-A7C81D8F794C}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -10566,7 +11661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1975A502-7E7F-4553-BC06-71CD8A16214F}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -10772,7 +11867,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FB9B18-434F-4677-A182-407CBC10EA8F}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -10993,729 +12088,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9F8961-463F-4540-AE96-5FF353928741}">
-  <sheetPr>
-    <tabColor theme="9" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:Q16"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.90625" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.1796875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="18.7265625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" s="16" customFormat="1" ht="87.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="43" t="s">
-        <v>278</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="48" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
-        <v>279</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="57">
-        <v>1</v>
-      </c>
-      <c r="I2" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="58"/>
-      <c r="L2" s="58">
-        <v>1</v>
-      </c>
-      <c r="M2" s="59">
-        <v>4</v>
-      </c>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59">
-        <v>10</v>
-      </c>
-      <c r="P2" s="59"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="60">
-        <v>1</v>
-      </c>
-      <c r="I3" s="61" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="24"/>
-      <c r="L3" s="24">
-        <v>1</v>
-      </c>
-      <c r="M3" s="62">
-        <v>2</v>
-      </c>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62">
-        <v>30</v>
-      </c>
-      <c r="P3" s="62"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>264</v>
-      </c>
-      <c r="C4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="60">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" s="24"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="24">
-        <v>1</v>
-      </c>
-      <c r="M4" s="62">
-        <v>3</v>
-      </c>
-      <c r="N4" s="62"/>
-      <c r="O4" s="63">
-        <v>5</v>
-      </c>
-      <c r="P4" s="63"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>265</v>
-      </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" s="60">
-        <v>1</v>
-      </c>
-      <c r="I5" s="61" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="24">
-        <v>1</v>
-      </c>
-      <c r="M5" s="62">
-        <v>4</v>
-      </c>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62">
-        <v>5</v>
-      </c>
-      <c r="P5" s="62"/>
-    </row>
-    <row r="6" spans="1:17" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="64" t="s">
-        <v>279</v>
-      </c>
-      <c r="B6" s="65" t="s">
-        <v>266</v>
-      </c>
-      <c r="C6" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="67" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="68" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="69">
-        <v>1</v>
-      </c>
-      <c r="I6" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="71"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="71">
-        <v>1</v>
-      </c>
-      <c r="M6" s="72">
-        <v>1</v>
-      </c>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72">
-        <v>5</v>
-      </c>
-      <c r="P6" s="72"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>280</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="39">
-        <v>3.0680000000000001</v>
-      </c>
-      <c r="I7" t="s">
-        <v>289</v>
-      </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="42">
-        <v>0.98</v>
-      </c>
-      <c r="M7" s="40">
-        <v>1</v>
-      </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="40">
-        <v>5</v>
-      </c>
-      <c r="P7" s="40"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>280</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>271</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="39">
-        <v>0.46090000000000003</v>
-      </c>
-      <c r="I8" t="s">
-        <v>113</v>
-      </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="42">
-        <v>0.98</v>
-      </c>
-      <c r="M8" s="40">
-        <v>2</v>
-      </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="40">
-        <v>5</v>
-      </c>
-      <c r="P8" s="40"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>280</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>269</v>
-      </c>
-      <c r="C9" t="s">
-        <v>288</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="39">
-        <v>0.36799999999999999</v>
-      </c>
-      <c r="I9" t="s">
-        <v>148</v>
-      </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="42">
-        <v>0.98</v>
-      </c>
-      <c r="M9" s="40">
-        <v>2</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="40">
-        <v>5</v>
-      </c>
-      <c r="P9" s="40"/>
-    </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>280</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>267</v>
-      </c>
-      <c r="C10" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="39">
-        <v>0.27813253012048195</v>
-      </c>
-      <c r="I10" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="9">
-        <v>1</v>
-      </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8">
-        <v>4</v>
-      </c>
-      <c r="O10" s="8">
-        <v>5</v>
-      </c>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="52" t="s">
-        <v>281</v>
-      </c>
-      <c r="B11" s="53" t="s">
-        <v>268</v>
-      </c>
-      <c r="C11" s="54" t="s">
-        <v>285</v>
-      </c>
-      <c r="D11" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="55" t="s">
-        <v>173</v>
-      </c>
-      <c r="F11" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="57">
-        <v>2.0927000000000001E-4</v>
-      </c>
-      <c r="I11" s="54" t="s">
-        <v>286</v>
-      </c>
-      <c r="J11" s="58">
-        <v>4</v>
-      </c>
-      <c r="K11" s="54" t="s">
-        <v>276</v>
-      </c>
-      <c r="L11" s="58">
-        <v>0.90986310592664843</v>
-      </c>
-      <c r="M11" s="59">
-        <v>1</v>
-      </c>
-      <c r="N11" s="59"/>
-      <c r="O11" s="59">
-        <v>5</v>
-      </c>
-      <c r="P11" s="59"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>284</v>
-      </c>
-      <c r="C12" t="s">
-        <v>282</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="73">
-        <v>3.6788000000000001E-2</v>
-      </c>
-      <c r="I12" t="s">
-        <v>148</v>
-      </c>
-      <c r="J12" s="24">
-        <v>4</v>
-      </c>
-      <c r="K12" t="s">
-        <v>276</v>
-      </c>
-      <c r="L12" s="24">
-        <v>1</v>
-      </c>
-      <c r="M12" s="62">
-        <v>1</v>
-      </c>
-      <c r="N12" s="62"/>
-      <c r="O12" s="62">
-        <v>5</v>
-      </c>
-      <c r="P12" s="62"/>
-    </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>281</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>298</v>
-      </c>
-      <c r="C13" t="s">
-        <v>158</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="H13" s="39">
-        <v>4.7E-2</v>
-      </c>
-      <c r="I13" s="41" t="s">
-        <v>161</v>
-      </c>
-      <c r="J13" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="K13" s="41" t="s">
-        <v>277</v>
-      </c>
-      <c r="L13" s="9">
-        <v>1</v>
-      </c>
-      <c r="M13" s="8">
-        <v>2</v>
-      </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8">
-        <v>10</v>
-      </c>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="52" t="s">
-        <v>287</v>
-      </c>
-      <c r="B14" s="53" t="s">
-        <v>272</v>
-      </c>
-      <c r="C14" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="D14" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="55" t="s">
-        <v>173</v>
-      </c>
-      <c r="F14" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="57">
-        <v>3.3109200000000005E-2</v>
-      </c>
-      <c r="I14" s="54" t="s">
-        <v>148</v>
-      </c>
-      <c r="J14" s="58"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="58">
-        <v>0.87556301899925537</v>
-      </c>
-      <c r="M14" s="59">
-        <v>1</v>
-      </c>
-      <c r="N14" s="59"/>
-      <c r="O14" s="59">
-        <v>10</v>
-      </c>
-      <c r="P14" s="59"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>273</v>
-      </c>
-      <c r="C15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="60">
-        <v>3.3109200000000005E-2</v>
-      </c>
-      <c r="I15" t="s">
-        <v>148</v>
-      </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="24">
-        <v>0.87556301899925537</v>
-      </c>
-      <c r="M15" s="62">
-        <v>1</v>
-      </c>
-      <c r="N15" s="62"/>
-      <c r="O15" s="62">
-        <v>10</v>
-      </c>
-      <c r="P15" s="62"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="J16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1E3EE0E1-6392-4754-984C-80D83AFED092}">
-          <x14:formula1>
-            <xm:f>Lookup!$D$2:$D$15</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F9 F11:F15 F17:F332</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{925A0EEB-9365-4265-BCAA-8FCF4189DF40}">
-          <x14:formula1>
-            <xm:f>Lookup!$B$2:$B$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E15 E17:E233</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C319048F-06A6-4121-9C15-D4FC96370093}">
-          <x14:formula1>
-            <xm:f>Lookup!$F$2:$F$45</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G15 G17:G1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update inputs files to include coverage rates tab
Coverage rates tab is added to both Model_inputs.xlsx and Model_inputs_demo.xlsx. Additional column for coverage rates sheet on scenario tab.
</commit_message>
<xml_diff>
--- a/config/model_inputs_demo.xlsx
+++ b/config/model_inputs_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/rui_han_gatesfoundation_org/Documents/Documents/GitHub/Ethiopia-HEP-Capacity-Analysis/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="286" documentId="13_ncr:1_{7CCCDFD1-E59D-423C-8BB5-C2031FD3030E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{759DB3FD-D57C-4A43-97B2-53A3A60D15C6}"/>
+  <xr:revisionPtr revIDLastSave="306" documentId="13_ncr:1_{7CCCDFD1-E59D-423C-8BB5-C2031FD3030E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8628A7B7-DDEA-4CB6-8109-9EB6023E48B4}"/>
   <bookViews>
-    <workbookView xWindow="6390" yWindow="-21030" windowWidth="32880" windowHeight="18390" tabRatio="830" activeTab="12" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
+    <workbookView xWindow="2145" yWindow="-17955" windowWidth="41010" windowHeight="15240" tabRatio="830" activeTab="1" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="77" r:id="rId1"/>
@@ -24,15 +24,16 @@
     <sheet name="SeasonalityOffsets" sheetId="66" r:id="rId9"/>
     <sheet name="TaskValues_basic" sheetId="83" r:id="rId10"/>
     <sheet name="TaskValues_expanded" sheetId="109" r:id="rId11"/>
-    <sheet name="TaskAllocationByCadre" sheetId="97" r:id="rId12"/>
-    <sheet name="CadreRoles" sheetId="111" r:id="rId13"/>
-    <sheet name="CadreRoles_v0" sheetId="108" r:id="rId14"/>
-    <sheet name="Data dictionary Scenarios" sheetId="63" r:id="rId15"/>
-    <sheet name="Lookup" sheetId="84" r:id="rId16"/>
+    <sheet name="CoverageRates" sheetId="113" r:id="rId12"/>
+    <sheet name="TaskAllocationByCadre" sheetId="97" r:id="rId13"/>
+    <sheet name="CadreRoles" sheetId="111" r:id="rId14"/>
+    <sheet name="CadreRoles_v0" sheetId="108" r:id="rId15"/>
+    <sheet name="Data dictionary Scenarios" sheetId="63" r:id="rId16"/>
+    <sheet name="Lookup" sheetId="84" r:id="rId17"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId17"/>
     <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TaskValues_basic!$B$1:$Q$15</definedName>
@@ -82,6 +83,7 @@
     <author>tc={81CABEFC-7899-4C7A-B9AE-4E2D5F662376}</author>
     <author>tc={014F1C08-667B-46ED-851F-81B8588E32D0}</author>
     <author>tc={4CC0DF8F-AAA1-4EBE-B532-0D230C5FDFB7}</author>
+    <author>tc={E0287D98-688F-4109-B85D-5FB1C1026365}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{328CAD55-03AD-4788-A8E4-651178ABBA8A}">
@@ -172,6 +174,14 @@
     The exact name (including capitalization) of a tab in this workbook that contains the cadre task allocations. Can be one or multiple tabs, but only one is used per scenario run.</t>
       </text>
     </comment>
+    <comment ref="M1" authorId="11" shapeId="0" xr:uid="{E0287D98-688F-4109-B85D-5FB1C1026365}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The exact name (including capitalization) of a tab in this workbook that contains the task-specific coverage rates. Can be one or multiple tabs, but only one is used per scenario run.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -234,8 +244,42 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Rui Han (AgileOne)</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{3AB316E4-10F3-4507-B0EF-A22783A43FA9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rui Han (AgileOne):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If these are left blank or a task is not included on this sheet, it will be assumed to be 100% coverage.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="347">
   <si>
     <t>Pregnancy</t>
   </si>
@@ -1207,6 +1251,75 @@
   </si>
   <si>
     <t>Format update date: 6/2/2023.</t>
+  </si>
+  <si>
+    <t>sheet_Coverage</t>
+  </si>
+  <si>
+    <t>CoverageRates</t>
+  </si>
+  <si>
+    <t>Year 0</t>
+  </si>
+  <si>
+    <t>Year 1</t>
+  </si>
+  <si>
+    <t>Year 2</t>
+  </si>
+  <si>
+    <t>Year 3</t>
+  </si>
+  <si>
+    <t>Year 4</t>
+  </si>
+  <si>
+    <t>Year 5</t>
+  </si>
+  <si>
+    <t>Year 6</t>
+  </si>
+  <si>
+    <t>Year 7</t>
+  </si>
+  <si>
+    <t>Year 8</t>
+  </si>
+  <si>
+    <t>Year 9</t>
+  </si>
+  <si>
+    <t>Year 10</t>
+  </si>
+  <si>
+    <t>Year 11</t>
+  </si>
+  <si>
+    <t>Year 12</t>
+  </si>
+  <si>
+    <t>Year 13</t>
+  </si>
+  <si>
+    <t>Year 14</t>
+  </si>
+  <si>
+    <t>Year 15</t>
+  </si>
+  <si>
+    <t>Year 16</t>
+  </si>
+  <si>
+    <t>Year 17</t>
+  </si>
+  <si>
+    <t>Year 18</t>
+  </si>
+  <si>
+    <t>Year 19</t>
+  </si>
+  <si>
+    <t>Year 20</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1334,7 @@
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1356,8 +1469,25 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1403,6 +1533,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1583,7 +1725,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1729,6 +1871,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="10" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="60" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2107,6 +2256,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Rui Han (AgileOne)" id="{9909CE15-4B7B-4B12-B2AC-B027CA4AD901}" userId="S::rui.han@gatesfoundation.org::8e2486fc-4f63-445b-b2ee-a849708c4214" providerId="AD"/>
   <person displayName="Brittany Hagedorn" id="{03786AFB-E7BB-4FA7-846C-835FB448EEBC}" userId="S::Brittany.Hagedorn@gatesfoundation.org::5a602c7b-e691-4c99-b6e7-afdfc0897536" providerId="AD"/>
 </personList>
 </file>
@@ -2441,6 +2591,9 @@
   <threadedComment ref="L1" dT="2022-11-12T18:37:39.80" personId="{03786AFB-E7BB-4FA7-846C-835FB448EEBC}" id="{4CC0DF8F-AAA1-4EBE-B532-0D230C5FDFB7}">
     <text>The exact name (including capitalization) of a tab in this workbook that contains the cadre task allocations. Can be one or multiple tabs, but only one is used per scenario run.</text>
   </threadedComment>
+  <threadedComment ref="M1" dT="2023-06-06T20:39:28.17" personId="{9909CE15-4B7B-4B12-B2AC-B027CA4AD901}" id="{E0287D98-688F-4109-B85D-5FB1C1026365}">
+    <text>The exact name (including capitalization) of a tab in this workbook that contains the task-specific coverage rates. Can be one or multiple tabs, but only one is used per scenario run.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2534,7 +2687,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3259,7 +3412,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4329,6 +4482,413 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F852F6A3-2ADB-4C94-AD23-1F9CFA07C02D}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:W21"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" style="105" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.81640625" style="105" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="6" style="105" bestFit="1" customWidth="1"/>
+    <col min="13" max="23" width="7" style="105" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.7265625" style="105"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="104" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="103" t="s">
+        <v>326</v>
+      </c>
+      <c r="D1" s="103" t="s">
+        <v>327</v>
+      </c>
+      <c r="E1" s="103" t="s">
+        <v>328</v>
+      </c>
+      <c r="F1" s="103" t="s">
+        <v>329</v>
+      </c>
+      <c r="G1" s="103" t="s">
+        <v>330</v>
+      </c>
+      <c r="H1" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I1" s="103" t="s">
+        <v>332</v>
+      </c>
+      <c r="J1" s="103" t="s">
+        <v>333</v>
+      </c>
+      <c r="K1" s="103" t="s">
+        <v>334</v>
+      </c>
+      <c r="L1" s="103" t="s">
+        <v>335</v>
+      </c>
+      <c r="M1" s="103" t="s">
+        <v>336</v>
+      </c>
+      <c r="N1" s="103" t="s">
+        <v>337</v>
+      </c>
+      <c r="O1" s="103" t="s">
+        <v>338</v>
+      </c>
+      <c r="P1" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q1" s="103" t="s">
+        <v>340</v>
+      </c>
+      <c r="R1" s="103" t="s">
+        <v>341</v>
+      </c>
+      <c r="S1" s="103" t="s">
+        <v>342</v>
+      </c>
+      <c r="T1" s="103" t="s">
+        <v>343</v>
+      </c>
+      <c r="U1" s="103" t="s">
+        <v>344</v>
+      </c>
+      <c r="V1" s="103" t="s">
+        <v>345</v>
+      </c>
+      <c r="W1" s="103" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" s="105" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="105" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:G3" si="0">C2</f>
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:L3" si="1">0.75</f>
+        <v>0.75</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="M2">
+        <v>0.9</v>
+      </c>
+      <c r="N2">
+        <v>0.9</v>
+      </c>
+      <c r="O2">
+        <v>0.9</v>
+      </c>
+      <c r="P2">
+        <v>0.9</v>
+      </c>
+      <c r="Q2">
+        <v>0.9</v>
+      </c>
+      <c r="R2">
+        <v>0.95</v>
+      </c>
+      <c r="S2">
+        <v>0.95</v>
+      </c>
+      <c r="T2">
+        <v>0.95</v>
+      </c>
+      <c r="U2">
+        <v>0.95</v>
+      </c>
+      <c r="V2">
+        <v>0.95</v>
+      </c>
+      <c r="W2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" s="105" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="105" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="M3">
+        <v>0.9</v>
+      </c>
+      <c r="N3">
+        <v>0.9</v>
+      </c>
+      <c r="O3">
+        <v>0.9</v>
+      </c>
+      <c r="P3">
+        <v>0.9</v>
+      </c>
+      <c r="Q3">
+        <v>0.9</v>
+      </c>
+      <c r="R3">
+        <v>0.95</v>
+      </c>
+      <c r="S3">
+        <v>0.95</v>
+      </c>
+      <c r="T3">
+        <v>0.95</v>
+      </c>
+      <c r="U3">
+        <v>0.95</v>
+      </c>
+      <c r="V3">
+        <v>0.95</v>
+      </c>
+      <c r="W3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="105" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" s="105" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" s="105" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" s="105" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="105" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" s="105" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" s="105" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" s="105" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" s="105" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" s="105" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10" s="105" t="s">
+        <v>267</v>
+      </c>
+      <c r="B10" s="105" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A11" s="105" t="s">
+        <v>268</v>
+      </c>
+      <c r="B11" s="105" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A12" s="105" t="s">
+        <v>284</v>
+      </c>
+      <c r="B12" s="105" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A13" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" s="105" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="B14" s="105" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A15" s="105" t="s">
+        <v>273</v>
+      </c>
+      <c r="B15" s="105" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" s="105" t="s">
+        <v>290</v>
+      </c>
+      <c r="B16" s="105" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="105" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" s="105" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="105" t="s">
+        <v>292</v>
+      </c>
+      <c r="B18" s="105" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="105" t="s">
+        <v>294</v>
+      </c>
+      <c r="B19" s="105" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="105" t="s">
+        <v>295</v>
+      </c>
+      <c r="B20" s="105" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="105" t="s">
+        <v>293</v>
+      </c>
+      <c r="B21" s="105" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:W3" xr:uid="{F44FB59B-9615-4BA6-B156-12EF80F548EA}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04D6E33-24B9-46AB-8C0C-B9AE70A8D6D8}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -5708,14 +6268,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A266884E-25A4-43DE-83DF-867907ACC671}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -5944,7 +6504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54E086A-5AFA-4FBE-A195-2972B691F429}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -6180,7 +6740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88F02ED-B255-4EEF-8CAA-1A7122B8C9FB}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -6310,7 +6870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2681DF91-CB0A-43E1-9090-E7803F99E625}">
   <dimension ref="B1:L142"/>
   <sheetViews>
@@ -7436,8 +7996,8 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7492,7 +8052,9 @@
       <c r="L1" s="83" t="s">
         <v>170</v>
       </c>
-      <c r="M1"/>
+      <c r="M1" s="106" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
@@ -7531,6 +8093,9 @@
       <c r="L2" s="5" t="s">
         <v>317</v>
       </c>
+      <c r="M2" s="107" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
@@ -7569,6 +8134,9 @@
       <c r="L3" s="5" t="s">
         <v>317</v>
       </c>
+      <c r="M3" s="107" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
@@ -7606,6 +8174,9 @@
       </c>
       <c r="L4" s="5" t="s">
         <v>317</v>
+      </c>
+      <c r="M4" s="107" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update inputs files to be compatible with new features
New features are: ChangeRateLimites and coverage rates.
</commit_message>
<xml_diff>
--- a/config/model_inputs_demo.xlsx
+++ b/config/model_inputs_demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\Ethiopia-HEP-Capacity-Analysis\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E62E3C-36BE-4900-900A-DAABC854405E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11B3F6A-EBF6-413A-8569-5DC70F7A3733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1030" yWindow="650" windowWidth="28770" windowHeight="11090" tabRatio="830" activeTab="3" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="830" activeTab="3" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="77" r:id="rId1"/>
@@ -24,15 +24,16 @@
     <sheet name="SeasonalityOffsets" sheetId="66" r:id="rId9"/>
     <sheet name="TaskValues_basic" sheetId="83" r:id="rId10"/>
     <sheet name="TaskValues_expanded" sheetId="109" r:id="rId11"/>
-    <sheet name="TaskAllocationByCadre" sheetId="97" r:id="rId12"/>
-    <sheet name="CadreRoles" sheetId="111" r:id="rId13"/>
-    <sheet name="CadreRoles_v0" sheetId="108" r:id="rId14"/>
-    <sheet name="Data dictionary Scenarios" sheetId="63" r:id="rId15"/>
-    <sheet name="Lookup" sheetId="84" r:id="rId16"/>
+    <sheet name="CoverageRates" sheetId="113" r:id="rId12"/>
+    <sheet name="TaskAllocationByCadre" sheetId="97" r:id="rId13"/>
+    <sheet name="CadreRoles" sheetId="111" r:id="rId14"/>
+    <sheet name="CadreRoles_v0" sheetId="108" r:id="rId15"/>
+    <sheet name="Data dictionary Scenarios" sheetId="63" r:id="rId16"/>
+    <sheet name="Lookup" sheetId="84" r:id="rId17"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId17"/>
     <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TaskValues_basic!$B$1:$Q$15</definedName>
@@ -82,6 +83,7 @@
     <author>tc={81CABEFC-7899-4C7A-B9AE-4E2D5F662376}</author>
     <author>tc={014F1C08-667B-46ED-851F-81B8588E32D0}</author>
     <author>tc={4CC0DF8F-AAA1-4EBE-B532-0D230C5FDFB7}</author>
+    <author>tc={E0287D98-688F-4109-B85D-5FB1C1026365}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{328CAD55-03AD-4788-A8E4-651178ABBA8A}">
@@ -172,6 +174,14 @@
     The exact name (including capitalization) of a tab in this workbook that contains the cadre task allocations. Can be one or multiple tabs, but only one is used per scenario run.</t>
       </text>
     </comment>
+    <comment ref="M1" authorId="11" shapeId="0" xr:uid="{E0287D98-688F-4109-B85D-5FB1C1026365}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The exact name (including capitalization) of a tab in this workbook that contains the task-specific coverage rates. Can be one or multiple tabs, but only one is used per scenario run.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -234,8 +244,42 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Rui Han (AgileOne)</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{3AB316E4-10F3-4507-B0EF-A22783A43FA9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rui Han (AgileOne):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If these are left blank or a task is not included on this sheet, it will be assumed to be 100% coverage.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="347">
   <si>
     <t>Pregnancy</t>
   </si>
@@ -1207,6 +1251,75 @@
   </si>
   <si>
     <t>Format update date: 6/2/2023.</t>
+  </si>
+  <si>
+    <t>sheet_Coverage</t>
+  </si>
+  <si>
+    <t>CoverageRates</t>
+  </si>
+  <si>
+    <t>Year 0</t>
+  </si>
+  <si>
+    <t>Year 1</t>
+  </si>
+  <si>
+    <t>Year 2</t>
+  </si>
+  <si>
+    <t>Year 3</t>
+  </si>
+  <si>
+    <t>Year 4</t>
+  </si>
+  <si>
+    <t>Year 5</t>
+  </si>
+  <si>
+    <t>Year 6</t>
+  </si>
+  <si>
+    <t>Year 7</t>
+  </si>
+  <si>
+    <t>Year 8</t>
+  </si>
+  <si>
+    <t>Year 9</t>
+  </si>
+  <si>
+    <t>Year 10</t>
+  </si>
+  <si>
+    <t>Year 11</t>
+  </si>
+  <si>
+    <t>Year 12</t>
+  </si>
+  <si>
+    <t>Year 13</t>
+  </si>
+  <si>
+    <t>Year 14</t>
+  </si>
+  <si>
+    <t>Year 15</t>
+  </si>
+  <si>
+    <t>Year 16</t>
+  </si>
+  <si>
+    <t>Year 17</t>
+  </si>
+  <si>
+    <t>Year 18</t>
+  </si>
+  <si>
+    <t>Year 19</t>
+  </si>
+  <si>
+    <t>Year 20</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1334,7 @@
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1356,8 +1469,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1403,6 +1527,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1583,7 +1719,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1729,6 +1865,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="10" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="60" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2107,6 +2249,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Rui Han (AgileOne)" id="{9909CE15-4B7B-4B12-B2AC-B027CA4AD901}" userId="S::rui.han@gatesfoundation.org::8e2486fc-4f63-445b-b2ee-a849708c4214" providerId="AD"/>
   <person displayName="Brittany Hagedorn" id="{03786AFB-E7BB-4FA7-846C-835FB448EEBC}" userId="S::Brittany.Hagedorn@gatesfoundation.org::5a602c7b-e691-4c99-b6e7-afdfc0897536" providerId="AD"/>
 </personList>
 </file>
@@ -2441,6 +2584,9 @@
   <threadedComment ref="L1" dT="2022-11-12T18:37:39.80" personId="{03786AFB-E7BB-4FA7-846C-835FB448EEBC}" id="{4CC0DF8F-AAA1-4EBE-B532-0D230C5FDFB7}">
     <text>The exact name (including capitalization) of a tab in this workbook that contains the cadre task allocations. Can be one or multiple tabs, but only one is used per scenario run.</text>
   </threadedComment>
+  <threadedComment ref="M1" dT="2023-06-06T20:39:28.17" personId="{9909CE15-4B7B-4B12-B2AC-B027CA4AD901}" id="{E0287D98-688F-4109-B85D-5FB1C1026365}">
+    <text>The exact name (including capitalization) of a tab in this workbook that contains the task-specific coverage rates. Can be one or multiple tabs, but only one is used per scenario run.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2534,7 +2680,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3259,7 +3405,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4329,6 +4475,412 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F852F6A3-2ADB-4C94-AD23-1F9CFA07C02D}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:W21"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="23" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="104" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="103" t="s">
+        <v>326</v>
+      </c>
+      <c r="D1" s="103" t="s">
+        <v>327</v>
+      </c>
+      <c r="E1" s="103" t="s">
+        <v>328</v>
+      </c>
+      <c r="F1" s="103" t="s">
+        <v>329</v>
+      </c>
+      <c r="G1" s="103" t="s">
+        <v>330</v>
+      </c>
+      <c r="H1" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I1" s="103" t="s">
+        <v>332</v>
+      </c>
+      <c r="J1" s="103" t="s">
+        <v>333</v>
+      </c>
+      <c r="K1" s="103" t="s">
+        <v>334</v>
+      </c>
+      <c r="L1" s="103" t="s">
+        <v>335</v>
+      </c>
+      <c r="M1" s="103" t="s">
+        <v>336</v>
+      </c>
+      <c r="N1" s="103" t="s">
+        <v>337</v>
+      </c>
+      <c r="O1" s="103" t="s">
+        <v>338</v>
+      </c>
+      <c r="P1" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q1" s="103" t="s">
+        <v>340</v>
+      </c>
+      <c r="R1" s="103" t="s">
+        <v>341</v>
+      </c>
+      <c r="S1" s="103" t="s">
+        <v>342</v>
+      </c>
+      <c r="T1" s="103" t="s">
+        <v>343</v>
+      </c>
+      <c r="U1" s="103" t="s">
+        <v>344</v>
+      </c>
+      <c r="V1" s="103" t="s">
+        <v>345</v>
+      </c>
+      <c r="W1" s="103" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:G3" si="0">C2</f>
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:L3" si="1">0.75</f>
+        <v>0.75</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="M2">
+        <v>0.9</v>
+      </c>
+      <c r="N2">
+        <v>0.9</v>
+      </c>
+      <c r="O2">
+        <v>0.9</v>
+      </c>
+      <c r="P2">
+        <v>0.9</v>
+      </c>
+      <c r="Q2">
+        <v>0.9</v>
+      </c>
+      <c r="R2">
+        <v>0.95</v>
+      </c>
+      <c r="S2">
+        <v>0.95</v>
+      </c>
+      <c r="T2">
+        <v>0.95</v>
+      </c>
+      <c r="U2">
+        <v>0.95</v>
+      </c>
+      <c r="V2">
+        <v>0.95</v>
+      </c>
+      <c r="W2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="M3">
+        <v>0.9</v>
+      </c>
+      <c r="N3">
+        <v>0.9</v>
+      </c>
+      <c r="O3">
+        <v>0.9</v>
+      </c>
+      <c r="P3">
+        <v>0.9</v>
+      </c>
+      <c r="Q3">
+        <v>0.9</v>
+      </c>
+      <c r="R3">
+        <v>0.95</v>
+      </c>
+      <c r="S3">
+        <v>0.95</v>
+      </c>
+      <c r="T3">
+        <v>0.95</v>
+      </c>
+      <c r="U3">
+        <v>0.95</v>
+      </c>
+      <c r="V3">
+        <v>0.95</v>
+      </c>
+      <c r="W3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>267</v>
+      </c>
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>268</v>
+      </c>
+      <c r="B11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>284</v>
+      </c>
+      <c r="B12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>272</v>
+      </c>
+      <c r="B14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>273</v>
+      </c>
+      <c r="B15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>290</v>
+      </c>
+      <c r="B16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>292</v>
+      </c>
+      <c r="B18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B19" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>295</v>
+      </c>
+      <c r="B20" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>293</v>
+      </c>
+      <c r="B21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:W3" xr:uid="{F44FB59B-9615-4BA6-B156-12EF80F548EA}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04D6E33-24B9-46AB-8C0C-B9AE70A8D6D8}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -5708,7 +6260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A266884E-25A4-43DE-83DF-867907ACC671}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -5944,7 +6496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54E086A-5AFA-4FBE-A195-2972B691F429}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -6180,7 +6732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88F02ED-B255-4EEF-8CAA-1A7122B8C9FB}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -6310,7 +6862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2681DF91-CB0A-43E1-9090-E7803F99E625}">
   <dimension ref="B1:L142"/>
   <sheetViews>
@@ -7437,7 +7989,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L4"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7492,7 +8044,9 @@
       <c r="L1" s="83" t="s">
         <v>170</v>
       </c>
-      <c r="M1"/>
+      <c r="M1" s="105" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
@@ -7531,6 +8085,9 @@
       <c r="L2" s="5" t="s">
         <v>317</v>
       </c>
+      <c r="M2" s="106" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
@@ -7569,6 +8126,9 @@
       <c r="L3" s="5" t="s">
         <v>317</v>
       </c>
+      <c r="M3" s="106" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
@@ -7606,6 +8166,9 @@
       </c>
       <c r="L4" s="5" t="s">
         <v>317</v>
+      </c>
+      <c r="M4" s="106" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -8553,7 +9116,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
fixing and adding new regression tests
</commit_message>
<xml_diff>
--- a/config/model_inputs_demo.xlsx
+++ b/config/model_inputs_demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\Ethiopia-HEP-Capacity-Analysis\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11B3F6A-EBF6-413A-8569-5DC70F7A3733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2B757C-B76C-4E63-AFF6-4E5FB6B83359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="830" activeTab="3" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="9765" tabRatio="830" firstSheet="1" activeTab="1" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="77" r:id="rId1"/>
@@ -24,16 +24,17 @@
     <sheet name="SeasonalityOffsets" sheetId="66" r:id="rId9"/>
     <sheet name="TaskValues_basic" sheetId="83" r:id="rId10"/>
     <sheet name="TaskValues_expanded" sheetId="109" r:id="rId11"/>
-    <sheet name="CoverageRates" sheetId="113" r:id="rId12"/>
-    <sheet name="TaskAllocationByCadre" sheetId="97" r:id="rId13"/>
-    <sheet name="CadreRoles" sheetId="111" r:id="rId14"/>
-    <sheet name="CadreRoles_v0" sheetId="108" r:id="rId15"/>
-    <sheet name="Data dictionary Scenarios" sheetId="63" r:id="rId16"/>
-    <sheet name="Lookup" sheetId="84" r:id="rId17"/>
+    <sheet name="CoverageRates_step" sheetId="113" r:id="rId12"/>
+    <sheet name="CoverageRates" sheetId="114" r:id="rId13"/>
+    <sheet name="TaskAllocationByCadre" sheetId="97" r:id="rId14"/>
+    <sheet name="CadreRoles" sheetId="111" r:id="rId15"/>
+    <sheet name="CadreRoles_v0" sheetId="108" r:id="rId16"/>
+    <sheet name="Data dictionary Scenarios" sheetId="63" r:id="rId17"/>
+    <sheet name="Lookup" sheetId="84" r:id="rId18"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
+    <externalReference r:id="rId20"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TaskValues_basic!$B$1:$Q$15</definedName>
@@ -278,8 +279,42 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Rui Han (AgileOne)</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{CA017E4B-2D5B-4FF4-955D-34398DF7F06C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rui Han (AgileOne):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If these are left blank or a task is not included on this sheet, it will be assumed to be 100% coverage.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="349">
   <si>
     <t>Pregnancy</t>
   </si>
@@ -1256,70 +1291,76 @@
     <t>sheet_Coverage</t>
   </si>
   <si>
+    <t>Year 0</t>
+  </si>
+  <si>
+    <t>Year 1</t>
+  </si>
+  <si>
+    <t>Year 2</t>
+  </si>
+  <si>
+    <t>Year 3</t>
+  </si>
+  <si>
+    <t>Year 4</t>
+  </si>
+  <si>
+    <t>Year 5</t>
+  </si>
+  <si>
+    <t>Year 6</t>
+  </si>
+  <si>
+    <t>Year 7</t>
+  </si>
+  <si>
+    <t>Year 8</t>
+  </si>
+  <si>
+    <t>Year 9</t>
+  </si>
+  <si>
+    <t>Year 10</t>
+  </si>
+  <si>
+    <t>Year 11</t>
+  </si>
+  <si>
+    <t>Year 12</t>
+  </si>
+  <si>
+    <t>Year 13</t>
+  </si>
+  <si>
+    <t>Year 14</t>
+  </si>
+  <si>
+    <t>Year 15</t>
+  </si>
+  <si>
+    <t>Year 16</t>
+  </si>
+  <si>
+    <t>Year 17</t>
+  </si>
+  <si>
+    <t>Year 18</t>
+  </si>
+  <si>
+    <t>Year 19</t>
+  </si>
+  <si>
+    <t>Year 20</t>
+  </si>
+  <si>
     <t>CoverageRates</t>
   </si>
   <si>
-    <t>Year 0</t>
-  </si>
-  <si>
-    <t>Year 1</t>
-  </si>
-  <si>
-    <t>Year 2</t>
-  </si>
-  <si>
-    <t>Year 3</t>
-  </si>
-  <si>
-    <t>Year 4</t>
-  </si>
-  <si>
-    <t>Year 5</t>
-  </si>
-  <si>
-    <t>Year 6</t>
-  </si>
-  <si>
-    <t>Year 7</t>
-  </si>
-  <si>
-    <t>Year 8</t>
-  </si>
-  <si>
-    <t>Year 9</t>
-  </si>
-  <si>
-    <t>Year 10</t>
-  </si>
-  <si>
-    <t>Year 11</t>
-  </si>
-  <si>
-    <t>Year 12</t>
-  </si>
-  <si>
-    <t>Year 13</t>
-  </si>
-  <si>
-    <t>Year 14</t>
-  </si>
-  <si>
-    <t>Year 15</t>
-  </si>
-  <si>
-    <t>Year 16</t>
-  </si>
-  <si>
-    <t>Year 17</t>
-  </si>
-  <si>
-    <t>Year 18</t>
-  </si>
-  <si>
-    <t>Year 19</t>
-  </si>
-  <si>
-    <t>Year 20</t>
+    <t>StepCoverage</t>
+  </si>
+  <si>
+    <t>CoverageRates_step</t>
   </si>
 </sst>
 </file>
@@ -2678,7 +2719,7 @@
   </sheetPr>
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
@@ -4481,8 +4522,8 @@
   </sheetPr>
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4501,67 +4542,67 @@
         <v>37</v>
       </c>
       <c r="C1" s="103" t="s">
+        <v>325</v>
+      </c>
+      <c r="D1" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="E1" s="103" t="s">
         <v>327</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="F1" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="G1" s="103" t="s">
         <v>329</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="H1" s="103" t="s">
         <v>330</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="I1" s="103" t="s">
         <v>331</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="J1" s="103" t="s">
         <v>332</v>
       </c>
-      <c r="J1" s="103" t="s">
+      <c r="K1" s="103" t="s">
         <v>333</v>
       </c>
-      <c r="K1" s="103" t="s">
+      <c r="L1" s="103" t="s">
         <v>334</v>
       </c>
-      <c r="L1" s="103" t="s">
+      <c r="M1" s="103" t="s">
         <v>335</v>
       </c>
-      <c r="M1" s="103" t="s">
+      <c r="N1" s="103" t="s">
         <v>336</v>
       </c>
-      <c r="N1" s="103" t="s">
+      <c r="O1" s="103" t="s">
         <v>337</v>
       </c>
-      <c r="O1" s="103" t="s">
+      <c r="P1" s="103" t="s">
         <v>338</v>
       </c>
-      <c r="P1" s="103" t="s">
+      <c r="Q1" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="Q1" s="103" t="s">
+      <c r="R1" s="103" t="s">
         <v>340</v>
       </c>
-      <c r="R1" s="103" t="s">
+      <c r="S1" s="103" t="s">
         <v>341</v>
       </c>
-      <c r="S1" s="103" t="s">
+      <c r="T1" s="103" t="s">
         <v>342</v>
       </c>
-      <c r="T1" s="103" t="s">
+      <c r="U1" s="103" t="s">
         <v>343</v>
       </c>
-      <c r="U1" s="103" t="s">
+      <c r="V1" s="103" t="s">
         <v>344</v>
       </c>
-      <c r="V1" s="103" t="s">
+      <c r="W1" s="103" t="s">
         <v>345</v>
-      </c>
-      <c r="W1" s="103" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.35">
@@ -4572,76 +4613,68 @@
         <v>144</v>
       </c>
       <c r="C2">
+        <v>0.25</v>
+      </c>
+      <c r="D2">
+        <v>0.25</v>
+      </c>
+      <c r="E2">
+        <v>0.25</v>
+      </c>
+      <c r="F2">
+        <v>0.25</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2" si="0">F2</f>
+        <v>0.25</v>
+      </c>
+      <c r="H2">
         <v>0.5</v>
       </c>
-      <c r="D2">
-        <f t="shared" ref="D2:G3" si="0">C2</f>
+      <c r="I2">
         <v>0.5</v>
       </c>
-      <c r="E2">
-        <f t="shared" si="0"/>
+      <c r="J2">
         <v>0.5</v>
       </c>
-      <c r="F2">
-        <f t="shared" si="0"/>
+      <c r="K2">
         <v>0.5</v>
       </c>
-      <c r="G2">
-        <f t="shared" si="0"/>
+      <c r="L2">
         <v>0.5</v>
       </c>
-      <c r="H2">
-        <f t="shared" ref="H2:L3" si="1">0.75</f>
+      <c r="M2">
         <v>0.75</v>
       </c>
-      <c r="I2">
-        <f t="shared" si="1"/>
+      <c r="N2">
         <v>0.75</v>
       </c>
-      <c r="J2">
-        <f t="shared" si="1"/>
+      <c r="O2">
         <v>0.75</v>
       </c>
-      <c r="K2">
-        <f t="shared" si="1"/>
+      <c r="P2">
         <v>0.75</v>
       </c>
-      <c r="L2">
-        <f t="shared" si="1"/>
+      <c r="Q2">
         <v>0.75</v>
       </c>
-      <c r="M2">
-        <v>0.9</v>
-      </c>
-      <c r="N2">
-        <v>0.9</v>
-      </c>
-      <c r="O2">
-        <v>0.9</v>
-      </c>
-      <c r="P2">
-        <v>0.9</v>
-      </c>
-      <c r="Q2">
-        <v>0.9</v>
-      </c>
       <c r="R2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="S2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="V2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="W2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
@@ -4652,76 +4685,67 @@
         <v>99</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="Q3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="S3">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="U3">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="V3">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="W3">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
@@ -4826,6 +4850,21 @@
       </c>
       <c r="B16" t="s">
         <v>249</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+      <c r="E16">
+        <v>0.5</v>
+      </c>
+      <c r="F16">
+        <v>0.5</v>
+      </c>
+      <c r="G16">
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -4881,6 +4920,271 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1486908E-A1DC-49FC-8BDF-3898C0F86D25}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:W21"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="23" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="104" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="103" t="s">
+        <v>325</v>
+      </c>
+      <c r="D1" s="103" t="s">
+        <v>326</v>
+      </c>
+      <c r="E1" s="103" t="s">
+        <v>327</v>
+      </c>
+      <c r="F1" s="103" t="s">
+        <v>328</v>
+      </c>
+      <c r="G1" s="103" t="s">
+        <v>329</v>
+      </c>
+      <c r="H1" s="103" t="s">
+        <v>330</v>
+      </c>
+      <c r="I1" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="J1" s="103" t="s">
+        <v>332</v>
+      </c>
+      <c r="K1" s="103" t="s">
+        <v>333</v>
+      </c>
+      <c r="L1" s="103" t="s">
+        <v>334</v>
+      </c>
+      <c r="M1" s="103" t="s">
+        <v>335</v>
+      </c>
+      <c r="N1" s="103" t="s">
+        <v>336</v>
+      </c>
+      <c r="O1" s="103" t="s">
+        <v>337</v>
+      </c>
+      <c r="P1" s="103" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q1" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="R1" s="103" t="s">
+        <v>340</v>
+      </c>
+      <c r="S1" s="103" t="s">
+        <v>341</v>
+      </c>
+      <c r="T1" s="103" t="s">
+        <v>342</v>
+      </c>
+      <c r="U1" s="103" t="s">
+        <v>343</v>
+      </c>
+      <c r="V1" s="103" t="s">
+        <v>344</v>
+      </c>
+      <c r="W1" s="103" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>267</v>
+      </c>
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>268</v>
+      </c>
+      <c r="B11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>284</v>
+      </c>
+      <c r="B12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>272</v>
+      </c>
+      <c r="B14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>273</v>
+      </c>
+      <c r="B15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>290</v>
+      </c>
+      <c r="B16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>292</v>
+      </c>
+      <c r="B18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B19" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>295</v>
+      </c>
+      <c r="B20" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>293</v>
+      </c>
+      <c r="B21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:W3" xr:uid="{7DC5F91B-50AD-4CAB-9C06-CFEC5BFD011B}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04D6E33-24B9-46AB-8C0C-B9AE70A8D6D8}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -6260,7 +6564,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A266884E-25A4-43DE-83DF-867907ACC671}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -6496,7 +6800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54E086A-5AFA-4FBE-A195-2972B691F429}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -6732,7 +7036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88F02ED-B255-4EEF-8CAA-1A7122B8C9FB}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -6862,7 +7166,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2681DF91-CB0A-43E1-9090-E7803F99E625}">
   <dimension ref="B1:L142"/>
   <sheetViews>
@@ -7988,8 +8292,8 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8086,7 +8390,7 @@
         <v>317</v>
       </c>
       <c r="M2" s="106" t="s">
-        <v>325</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -8127,7 +8431,7 @@
         <v>317</v>
       </c>
       <c r="M3" s="106" t="s">
-        <v>325</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -8168,7 +8472,48 @@
         <v>317</v>
       </c>
       <c r="M4" s="106" t="s">
-        <v>325</v>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B5" s="27">
+        <v>48</v>
+      </c>
+      <c r="C5" s="27">
+        <v>32</v>
+      </c>
+      <c r="D5" s="27">
+        <v>5000</v>
+      </c>
+      <c r="E5" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>256</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="M5" s="106" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -9115,7 +9460,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>